<commit_message>
Actualizo código del CRM
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -70,10 +70,16 @@
     <t>C1001</t>
   </si>
   <si>
+    <t>C1002</t>
+  </si>
+  <si>
     <t>Sebastian Toro</t>
   </si>
   <si>
     <t>Bandian Torres</t>
+  </si>
+  <si>
+    <t>Tatiana Avila</t>
   </si>
   <si>
     <t>mundo E</t>
@@ -479,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -540,46 +546,46 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -587,22 +593,45 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: save local changes (gs credentials & diagnostics, misc fixes)
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -73,6 +73,9 @@
     <t>C1002</t>
   </si>
   <si>
+    <t>C1003</t>
+  </si>
+  <si>
     <t>Sebastian Toro</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
   </si>
   <si>
     <t>Tatiana Avila</t>
+  </si>
+  <si>
+    <t>hola</t>
   </si>
   <si>
     <t>mundo E</t>
@@ -485,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -546,46 +552,46 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -593,22 +599,22 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -616,22 +622,45 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: persist data folder changes (clientes, historial, docs)
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -76,6 +76,9 @@
     <t>C1003</t>
   </si>
   <si>
+    <t>C1004</t>
+  </si>
+  <si>
     <t>Sebastian Toro</t>
   </si>
   <si>
@@ -86,6 +89,9 @@
   </si>
   <si>
     <t>hola</t>
+  </si>
+  <si>
+    <t>SAUL TORRES</t>
   </si>
   <si>
     <t>mundo E</t>
@@ -491,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -552,46 +558,46 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -599,22 +605,22 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -622,22 +628,22 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -645,22 +651,45 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: persist data changes (user requested)
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -70,9 +70,6 @@
     <t>C1001</t>
   </si>
   <si>
-    <t>C1002</t>
-  </si>
-  <si>
     <t>C1003</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
   </si>
   <si>
     <t>Bandian Torres</t>
-  </si>
-  <si>
-    <t>Tatiana Avila</t>
   </si>
   <si>
     <t>hola</t>
@@ -497,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -558,46 +552,46 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
       <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
       <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>36</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>37</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>38</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>39</v>
-      </c>
-      <c r="O2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -605,22 +599,22 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -628,22 +622,22 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -651,45 +645,22 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data: persist cambios en clientes, historial y docs
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -76,6 +76,9 @@
     <t>C1004</t>
   </si>
   <si>
+    <t>C1005</t>
+  </si>
+  <si>
     <t>Sebastian Toro</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
     <t>SAUL TORRES</t>
   </si>
   <si>
+    <t>VioletaAvila</t>
+  </si>
+  <si>
     <t>mundo E</t>
   </si>
   <si>
@@ -101,6 +107,9 @@
   </si>
   <si>
     <t>2025-10-08</t>
+  </si>
+  <si>
+    <t>2025-10-09</t>
   </si>
   <si>
     <t>2025-10-06</t>
@@ -491,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -552,46 +561,46 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="P2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -599,22 +608,22 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -622,22 +631,22 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -645,22 +654,45 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="E6" t="s">
         <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>